<commit_message>
Draft: Add collapsible schedule
</commit_message>
<xml_diff>
--- a/_data/program/program_rse24.xlsx
+++ b/_data/program/program_rse24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/argen/100 Projects/rse2024/rse2024-website/_data/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10B7D6F-36FC-204E-B287-812E84D00FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F5BDC1-5819-834B-98B9-5737B3B3BE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="3" xr2:uid="{1A9D135E-AEEF-714C-873D-A39C4189092C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="2" xr2:uid="{1A9D135E-AEEF-714C-873D-A39C4189092C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="294">
   <si>
     <t>Timestamp</t>
   </si>
@@ -946,6 +946,48 @@
   </si>
   <si>
     <t>Robotic Systems deal with many uncertainties which may hamper the operability and achievability of a mission. Robots need to be autonomous but also be able to reliably achieve an objective. In that sense, robotic systems offer great scenarios for requirement specification and verification. The challenge lies in precisely modelling adaptability within the system and verifying adaptable requirements at runtime. To that end, we propose an event based approach to runtime verification for ROS2 based systems that aims to bridge the gap between dynamic requirements specification and runtime verification by monitoring the state of the system and creating discrete events which are sent to a mission controller.</t>
+  </si>
+  <si>
+    <t>Professor of Computer Science</t>
+  </si>
+  <si>
+    <t>Co-Founder and Managing Director</t>
+  </si>
+  <si>
+    <t>Malte Langosz</t>
+  </si>
+  <si>
+    <t>Team Lead Software Backbone at the Robotics Innovation Center</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Ringo</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>Lyricist</t>
+  </si>
+  <si>
+    <t>Composer and base player</t>
+  </si>
+  <si>
+    <t>The Beatles</t>
+  </si>
+  <si>
+    <t>Composer and guitar player</t>
+  </si>
+  <si>
+    <t>Drum player</t>
   </si>
 </sst>
 </file>
@@ -1436,11 +1478,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RSE'24 - Submission Form (Responses) - Form Responses 1" connectionId="1" xr16:uid="{DF670F3A-DC84-6B4D-B657-B744C2C0C6DE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RSE_24___Submission_Form__Responses____Form_Responses_1_3" connectionId="1" xr16:uid="{F9E0855D-1C5D-2F41-BF2E-51700D4CFA07}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RSE_24___Submission_Form__Responses____Form_Responses_1_3" connectionId="1" xr16:uid="{F9E0855D-1C5D-2F41-BF2E-51700D4CFA07}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RSE'24 - Submission Form (Responses) - Form Responses 1" connectionId="1" xr16:uid="{DF670F3A-DC84-6B4D-B657-B744C2C0C6DE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2880,7 +2922,7 @@
   <dimension ref="B1:M63"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2972,6 +3014,9 @@
       <c r="C3" t="s">
         <v>174</v>
       </c>
+      <c r="D3" t="s">
+        <v>280</v>
+      </c>
       <c r="E3" s="17" t="s">
         <v>22</v>
       </c>
@@ -3106,9 +3151,15 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>289</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
@@ -3133,9 +3184,15 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
@@ -3160,9 +3217,15 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>292</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
@@ -3187,9 +3250,15 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
@@ -3703,13 +3772,13 @@
     </row>
     <row r="30" spans="2:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>23</v>
+        <v>282</v>
       </c>
       <c r="C30" t="s">
         <v>221</v>
       </c>
       <c r="D30" t="s">
-        <v>220</v>
+        <v>283</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>22</v>
@@ -3799,6 +3868,9 @@
       </c>
       <c r="C33" t="s">
         <v>222</v>
+      </c>
+      <c r="D33" t="s">
+        <v>281</v>
       </c>
       <c r="E33" s="17" t="s">
         <v>22</v>
@@ -4640,7 +4712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799E3A7E-32E2-2E44-B86D-9371E1932546}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
@@ -4755,7 +4827,7 @@
       </c>
       <c r="D3" t="str">
         <f>IF(ISBLANK(Schedule!D3),"",Schedule!D3)</f>
-        <v/>
+        <v>Professor of Computer Science</v>
       </c>
       <c r="E3" t="str">
         <f>IF(ISBLANK(Schedule!E3),"",Schedule!E3)</f>
@@ -4977,15 +5049,15 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8" t="str">
         <f>IF(ISBLANK(Schedule!B8),"",Schedule!B8)</f>
-        <v/>
+        <v>John</v>
       </c>
       <c r="C8" t="str">
         <f>IF(ISBLANK(Schedule!C8),"",Schedule!C8)</f>
-        <v/>
+        <v>NY</v>
       </c>
       <c r="D8" t="str">
         <f>IF(ISBLANK(Schedule!D8),"",Schedule!D8)</f>
-        <v/>
+        <v>Lyricist</v>
       </c>
       <c r="E8" t="str">
         <f>IF(ISBLANK(Schedule!E8),"",Schedule!E8)</f>
@@ -5023,15 +5095,15 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9" t="str">
         <f>IF(ISBLANK(Schedule!B9),"",Schedule!B9)</f>
-        <v/>
+        <v>Paul</v>
       </c>
       <c r="C9" t="str">
         <f>IF(ISBLANK(Schedule!C9),"",Schedule!C9)</f>
-        <v/>
+        <v>The Beatles</v>
       </c>
       <c r="D9" t="str">
         <f>IF(ISBLANK(Schedule!D9),"",Schedule!D9)</f>
-        <v/>
+        <v>Composer and base player</v>
       </c>
       <c r="E9" t="str">
         <f>IF(ISBLANK(Schedule!E9),"",Schedule!E9)</f>
@@ -5069,15 +5141,15 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" t="str">
         <f>IF(ISBLANK(Schedule!B10),"",Schedule!B10)</f>
-        <v/>
+        <v>George</v>
       </c>
       <c r="C10" t="str">
         <f>IF(ISBLANK(Schedule!C10),"",Schedule!C10)</f>
-        <v/>
+        <v>The Beatles</v>
       </c>
       <c r="D10" t="str">
         <f>IF(ISBLANK(Schedule!D10),"",Schedule!D10)</f>
-        <v/>
+        <v>Composer and guitar player</v>
       </c>
       <c r="E10" t="str">
         <f>IF(ISBLANK(Schedule!E10),"",Schedule!E10)</f>
@@ -5115,15 +5187,15 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B11" t="str">
         <f>IF(ISBLANK(Schedule!B11),"",Schedule!B11)</f>
-        <v/>
+        <v>Ringo</v>
       </c>
       <c r="C11" t="str">
         <f>IF(ISBLANK(Schedule!C11),"",Schedule!C11)</f>
-        <v/>
+        <v>The Beatles</v>
       </c>
       <c r="D11" t="str">
         <f>IF(ISBLANK(Schedule!D11),"",Schedule!D11)</f>
-        <v/>
+        <v>Drum player</v>
       </c>
       <c r="E11" t="str">
         <f>IF(ISBLANK(Schedule!E11),"",Schedule!E11)</f>
@@ -5989,7 +6061,7 @@
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30" t="str">
         <f>IF(ISBLANK(Schedule!B30),"",Schedule!B30)</f>
-        <v>Malte Langosch</v>
+        <v>Malte Langosz</v>
       </c>
       <c r="C30" t="str">
         <f>IF(ISBLANK(Schedule!C30),"",Schedule!C30)</f>
@@ -5997,7 +6069,7 @@
       </c>
       <c r="D30" t="str">
         <f>IF(ISBLANK(Schedule!D30),"",Schedule!D30)</f>
-        <v>Team Lead Software Backbone</v>
+        <v>Team Lead Software Backbone at the Robotics Innovation Center</v>
       </c>
       <c r="E30" t="str">
         <f>IF(ISBLANK(Schedule!E30),"",Schedule!E30)</f>
@@ -6135,7 +6207,7 @@
       </c>
       <c r="D33" t="str">
         <f>IF(ISBLANK(Schedule!D33),"",Schedule!D33)</f>
-        <v/>
+        <v>Co-Founder and Managing Director</v>
       </c>
       <c r="E33" t="str">
         <f>IF(ISBLANK(Schedule!E33),"",Schedule!E33)</f>
@@ -7559,7 +7631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E4CC41-86B0-9149-8264-D6DA047BAB5C}">
   <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>

</xml_diff>